<commit_message>
First Version with pages
</commit_message>
<xml_diff>
--- a/data/TeamScores.xlsx
+++ b/data/TeamScores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrice/Documents/git/HealthyLifeFrontend01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA57A75-8F9E-E248-9FD3-9F81DD1E6A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BCEC1F-2822-8042-8221-52D45DCEBDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{4229BDAA-6B11-BA4B-B194-8D2473EE0840}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Team</t>
   </si>
@@ -45,6 +45,18 @@
   </si>
   <si>
     <t>Muchachos</t>
+  </si>
+  <si>
+    <t>Muchacho1</t>
+  </si>
+  <si>
+    <t>Bonjour1</t>
+  </si>
+  <si>
+    <t>Bonjour2</t>
+  </si>
+  <si>
+    <t>Muchacho2</t>
   </si>
 </sst>
 </file>
@@ -417,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F21C894E-3D0B-F74E-B5AD-3ED5D0BE7B71}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,6 +569,86 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>